<commit_message>
Coloquei dashboard, análise de quantidade de cada tipo e acurácia do programa
</commit_message>
<xml_diff>
--- a/NetflixNrt.xlsx
+++ b/NetflixNrt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projeto2-cdados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B377E9B-A67A-4F2B-8F44-B447DBFB0619}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238945E-30D0-4AD6-A447-95ED6EB5083E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="803">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2756,9 +2756,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -3173,7 +3170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L501"/>
   <sheetViews>
-    <sheetView topLeftCell="A422" workbookViewId="0">
+    <sheetView topLeftCell="A470" workbookViewId="0">
       <selection activeCell="D447" sqref="D447"/>
     </sheetView>
   </sheetViews>
@@ -7205,8 +7202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7500,7 +7497,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>537</v>
       </c>
       <c r="B37" s="4">
@@ -8152,7 +8149,7 @@
         <v>618</v>
       </c>
       <c r="B118" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -8160,7 +8157,7 @@
         <v>619</v>
       </c>
       <c r="B119" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -8176,7 +8173,7 @@
         <v>621</v>
       </c>
       <c r="B121" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -8184,7 +8181,7 @@
         <v>622</v>
       </c>
       <c r="B122" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -8192,7 +8189,7 @@
         <v>623</v>
       </c>
       <c r="B123" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -8200,7 +8197,7 @@
         <v>624</v>
       </c>
       <c r="B124" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -8208,7 +8205,7 @@
         <v>625</v>
       </c>
       <c r="B125" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -8224,7 +8221,7 @@
         <v>627</v>
       </c>
       <c r="B127" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -8240,7 +8237,7 @@
         <v>629</v>
       </c>
       <c r="B129" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -8248,7 +8245,7 @@
         <v>630</v>
       </c>
       <c r="B130" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -8288,7 +8285,7 @@
         <v>635</v>
       </c>
       <c r="B135" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -8304,7 +8301,7 @@
         <v>637</v>
       </c>
       <c r="B137" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -8637,15 +8634,15 @@
         <v>678</v>
       </c>
       <c r="B179" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>679</v>
       </c>
-      <c r="B180" s="4" t="s">
-        <v>803</v>
+      <c r="B180" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>